<commit_message>
auto:rephrased two questions and made the date the last question in the create form
</commit_message>
<xml_diff>
--- a/config/forms/app/create.xlsx
+++ b/config/forms/app/create.xlsx
@@ -129,7 +129,13 @@
     <t>title</t>
   </si>
   <si>
-    <t>What is the title of the task?</t>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notes about this task:</t>
   </si>
   <si>
     <t>date</t>
@@ -138,13 +144,7 @@
     <t>reminder</t>
   </si>
   <si>
-    <t xml:space="preserve">When should a reminder appear in the task tab? </t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Notes about this task:</t>
+    <t xml:space="preserve">When should a reminder appear in your tasks? </t>
   </si>
   <si>
     <t>list_name</t>
@@ -1101,16 +1101,16 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1125,8 +1125,8 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>23</v>
+      <c r="A24" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>42</v>
@@ -1134,7 +1134,7 @@
       <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C2" s="15" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-02_15-12</v>
+        <v>2022-10-19_09-51</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
auto:Update Task form to make all fields required
</commit_message>
<xml_diff>
--- a/config/forms/app/create.xlsx
+++ b/config/forms/app/create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="106">
   <si>
     <t>type</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Task of the Person Creating Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
   </si>
   <si>
     <t>date</t>
@@ -2203,8 +2206,9 @@
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -2218,20 +2222,21 @@
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H46" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -2245,18 +2250,19 @@
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -2273,15 +2279,16 @@
         <v>24</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
@@ -2374,7 +2381,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2423,48 +2430,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="24" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-08-11_18-21</v>
+        <v>2024-11-21_11-43</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="3"/>
     </row>

</xml_diff>